<commit_message>
- import dichvu: add column {SoPhutThucHien}
</commit_message>
<xml_diff>
--- a/beautify_api/8.0.0/aspnet-core/src/BanHangBeautify.Web.Host/wwwroot/ImportExcelTemplate/HangHoa_DichVu_ImportTemplate.xlsx
+++ b/beautify_api/8.0.0/aspnet-core/src/BanHangBeautify.Web.Host/wwwroot/ImportExcelTemplate/HangHoa_DichVu_ImportTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code-manhld-github\beautify_app_flutter\beautify_api\8.0.0\aspnet-core\src\BanHangBeautify.Web.Host\wwwroot\ImportExcelTemplate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Download\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,8 +13,11 @@
   </bookViews>
   <sheets>
     <sheet name="DanhSachImport" sheetId="1" r:id="rId1"/>
-    <sheet name="Hướng dẫn" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="MaHangHoa">DanhSachImport!$B$2</definedName>
+    <definedName name="TenHangHoa">DanhSachImport!$C$2</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,153 +28,59 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
-  <si>
-    <t>Tên dịch vụ - Hàng hóa</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Giá bán</t>
   </si>
   <si>
-    <t xml:space="preserve">Loại </t>
-  </si>
-  <si>
-    <t>Số phút thực hiện</t>
-  </si>
-  <si>
-    <t>Danh sách dịch vụ hàng hóa import</t>
-  </si>
-  <si>
-    <t>Loại</t>
-  </si>
-  <si>
-    <t>Giá trị nhập</t>
-  </si>
-  <si>
-    <t>Cột nhập tương ứng nhập</t>
-  </si>
-  <si>
-    <t>Giá trị tương ứng</t>
-  </si>
-  <si>
-    <t>Nhập giá trị nếu đó là dịch vụ</t>
+    <t>Ghi chú</t>
+  </si>
+  <si>
+    <t>Mã dịch vụ</t>
+  </si>
+  <si>
+    <t>Tên nhóm dịch vụ</t>
+  </si>
+  <si>
+    <t>Phẩu thuật thẩm mỹ</t>
+  </si>
+  <si>
+    <t>Cắt tạo hình môi trái tim/môi</t>
+  </si>
+  <si>
+    <t>Tên dịch vụ (*)</t>
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>HH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> hoặc </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>DV</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> hoặc </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>CB</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>HH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">: loại là hàng hóa
+      <t xml:space="preserve">MẪU FILE IMPORT DANH MỤC DỊCH VỤ
 </t>
     </r>
     <r>
       <rPr>
-        <b/>
-        <sz val="11"/>
+        <i/>
+        <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="163"/>
       </rPr>
-      <t>DV</t>
+      <t>(*): cột có dấu * thì bắt buộc nhập</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">: loại là dịch vụ
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>CB</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> : là dịch vụ hoặc hàng hóa theo combo</t>
-    </r>
-  </si>
-  <si>
-    <t>Ghi chú</t>
-  </si>
-  <si>
-    <t>Mã dịch vụ - Hàng hóa</t>
+  </si>
+  <si>
+    <t>Xứ lý sẹo bằng tiểu phẫu</t>
+  </si>
+  <si>
+    <t>Phun xăm</t>
+  </si>
+  <si>
+    <t>Điêu khắc chân mày</t>
+  </si>
+  <si>
+    <t>Phun môi pha lê</t>
+  </si>
+  <si>
+    <t>Số phút thực hiện</t>
   </si>
 </sst>
 </file>
@@ -195,37 +104,44 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="18"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="163"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="163"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="163"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="163"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="163"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -239,11 +155,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5F5F5"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -275,44 +198,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFE6E6E6"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
-    <cellStyle name="Accent2" xfId="2" builtinId="33"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -591,110 +522,107 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G2"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="39.5703125" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" customWidth="1"/>
-    <col min="7" max="7" width="35.85546875" customWidth="1"/>
+    <col min="1" max="1" width="23" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="39.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="35.85546875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+    </row>
+    <row r="2" spans="1:6" s="4" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="C3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="6">
+        <v>12000000</v>
+      </c>
+      <c r="E3" s="6">
+        <v>120</v>
+      </c>
+      <c r="F3" s="6"/>
     </row>
-    <row r="2" spans="2:7" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>12</v>
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="6">
+        <v>15000000</v>
+      </c>
+      <c r="E4" s="6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C8:E10"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="9.140625" style="5"/>
-    <col min="3" max="3" width="24.5703125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="28.28515625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" style="5" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="5"/>
-  </cols>
-  <sheetData>
-    <row r="8" spans="3:5" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C8" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="3:5" ht="59.25" x14ac:dyDescent="0.2">
-      <c r="C9" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="3:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="C10" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
- importKhachHang: return ListError
</commit_message>
<xml_diff>
--- a/beautify_api/8.0.0/aspnet-core/src/BanHangBeautify.Web.Host/wwwroot/ImportExcelTemplate/HangHoa_DichVu_ImportTemplate.xlsx
+++ b/beautify_api/8.0.0/aspnet-core/src/BanHangBeautify.Web.Host/wwwroot/ImportExcelTemplate/HangHoa_DichVu_ImportTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Download\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SSOFT\Open beauty\lucky_beauty\beautify_api\8.0.0\aspnet-core\src\BanHangBeautify.Web.Host\wwwroot\ImportExcelTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -51,8 +51,42 @@
     <t>Tên dịch vụ (*)</t>
   </si>
   <si>
+    <t>Xứ lý sẹo bằng tiểu phẫu</t>
+  </si>
+  <si>
+    <t>Phun xăm</t>
+  </si>
+  <si>
+    <t>Điêu khắc chân mày</t>
+  </si>
+  <si>
+    <t>Phun môi pha lê</t>
+  </si>
+  <si>
+    <t>Số phút thực hiện</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">MẪU FILE IMPORT DANH MỤC DỊCH VỤ
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="163"/>
+      </rPr>
+      <t>MẪU FILE IMPORT DANH MỤC DỊCH VỤ</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -66,21 +100,6 @@
       </rPr>
       <t>(*): cột có dấu * thì bắt buộc nhập</t>
     </r>
-  </si>
-  <si>
-    <t>Xứ lý sẹo bằng tiểu phẫu</t>
-  </si>
-  <si>
-    <t>Phun xăm</t>
-  </si>
-  <si>
-    <t>Điêu khắc chân mày</t>
-  </si>
-  <si>
-    <t>Phun môi pha lê</t>
-  </si>
-  <si>
-    <t>Số phút thực hiện</t>
   </si>
 </sst>
 </file>
@@ -103,21 +122,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="163"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="163"/>
-    </font>
-    <font>
       <b/>
       <sz val="16"/>
       <color theme="1"/>
@@ -134,8 +138,23 @@
       <charset val="163"/>
     </font>
     <font>
-      <sz val="11"/>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="163"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="163"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="163"/>
@@ -214,32 +233,32 @@
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="4" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -525,55 +544,55 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="39.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23" style="5" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="39.5703125" style="5" customWidth="1"/>
     <col min="4" max="4" width="23.85546875" style="6" customWidth="1"/>
     <col min="5" max="5" width="24.5703125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="35.85546875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="6" width="35.85546875" style="5" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
+      <c r="A1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:6" s="4" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:6" s="11" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="6">
@@ -584,12 +603,12 @@
       </c>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>8</v>
+      <c r="C4" s="7" t="s">
+        <v>7</v>
       </c>
       <c r="D4" s="6">
         <v>15000000</v>
@@ -599,22 +618,22 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7">
+      <c r="A6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8">
         <v>30</v>
       </c>
     </row>

</xml_diff>